<commit_message>
duplicate changes, form feed
Signed-off-by: Jelte Dirks <j.dirks@outlook.com>
</commit_message>
<xml_diff>
--- a/formulieren/09000.xlsx
+++ b/formulieren/09000.xlsx
@@ -11,6 +11,7 @@
     <sheet name="09060" sheetId="6" r:id="rId6"/>
     <sheet name="09080" sheetId="7" r:id="rId7"/>
     <sheet name="09810" sheetId="8" r:id="rId8"/>
+    <sheet name="09081" sheetId="9" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -9560,4 +9561,1559 @@
     <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G67"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>omschrijving</v>
+      </c>
+      <c r="B1" t="str">
+        <v>inhoud</v>
+      </c>
+      <c r="C1" t="str">
+        <v>weergave</v>
+      </c>
+      <c r="D1" t="str">
+        <v>uitlijnen</v>
+      </c>
+      <c r="E1" t="str">
+        <v>regel verwijderen</v>
+      </c>
+      <c r="F1" t="str">
+        <v>regel template</v>
+      </c>
+      <c r="G1" t="str">
+        <v>A327</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Verzekerde Modules</v>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v>_x000c_35 Verzekerde Modules</v>
+      </c>
+      <c r="G2" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Soort verzekering</v>
+      </c>
+      <c r="B3" t="str">
+        <v>10142</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v>02 Soort verzekering         10142</v>
+      </c>
+      <c r="G3" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v>10142</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E4" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Gezinssamenstelling</v>
+      </c>
+      <c r="B5" t="str">
+        <v>10694</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v>03 Gezinssamenstelling       10694</v>
+      </c>
+      <c r="G5" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>10694</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E6" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Aantal artsen</v>
+      </c>
+      <c r="B7" t="str">
+        <v>13610</v>
+      </c>
+      <c r="C7" t="str">
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v>04 Aantal artsen             13610</v>
+      </c>
+      <c r="G7" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" t="str">
+        <v>13610</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E8" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Vrije advocaat keuze (VAK)</v>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v>06                           Vrije advocaat keuze (VAK)</v>
+      </c>
+      <c r="G9" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Verzekerd bedrag VAK</v>
+      </c>
+      <c r="B10" t="str">
+        <v>€ 10611</v>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v>07 Verzekerd bedrag VAK      € 10611</v>
+      </c>
+      <c r="G10" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>10611</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E11" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Eigen bijdrage VAK</v>
+      </c>
+      <c r="B12" t="str">
+        <v>€ 13616</v>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v>08 Eigen bijdrage VAK        € 13616</v>
+      </c>
+      <c r="G12" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v>13616</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E13" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Militair</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Ja                                                      81005</v>
+      </c>
+      <c r="C14" t="str">
+        <v/>
+      </c>
+      <c r="D14" t="str">
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v>09 Militair                  Ja                                                      81005</v>
+      </c>
+      <c r="G14" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <v>81005</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E15" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Lid van militaire vakbond</v>
+      </c>
+      <c r="B16" t="str">
+        <v>80991                                                       81005</v>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v>10 Lid van militaire vakbond 80991                                                       81005</v>
+      </c>
+      <c r="G16" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v>80991</v>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E17" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v>81005</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E18" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Onroerend goed object 1</v>
+      </c>
+      <c r="B19" t="str">
+        <v>80079 80095 86578</v>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v>12 Onroerend goed object 1   80079 80095 86578</v>
+      </c>
+      <c r="G19" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v>80079</v>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E20" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <v>80095</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E21" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <v>86578</v>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E22" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B23" t="str">
+        <v>80084 80090</v>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v>13                           80084 80090</v>
+      </c>
+      <c r="G23" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v/>
+      </c>
+      <c r="B24" t="str">
+        <v>80084</v>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E24" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+      <c r="G24" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v/>
+      </c>
+      <c r="B25" t="str">
+        <v>80090</v>
+      </c>
+      <c r="C25" t="str">
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E25" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Dekkingscombinatie</v>
+      </c>
+      <c r="B26" t="str">
+        <v>80732</v>
+      </c>
+      <c r="C26" t="str">
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <v>14 Dekkingscombinatie        80732</v>
+      </c>
+      <c r="G26" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v/>
+      </c>
+      <c r="B27" t="str">
+        <v>80732</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E27" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Herbouwwaarde</v>
+      </c>
+      <c r="B28" t="str">
+        <v>€ 80008</v>
+      </c>
+      <c r="C28" t="str">
+        <v/>
+      </c>
+      <c r="D28" t="str">
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <v/>
+      </c>
+      <c r="F28" t="str">
+        <v>15 Herbouwwaarde             € 80008</v>
+      </c>
+      <c r="G28" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v/>
+      </c>
+      <c r="B29" t="str">
+        <v>80008</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E29" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Huurwaarde</v>
+      </c>
+      <c r="B30" t="str">
+        <v>€ 84818</v>
+      </c>
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <v>16 Huurwaarde                € 84818</v>
+      </c>
+      <c r="G30" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v/>
+      </c>
+      <c r="B31" t="str">
+        <v>84818</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E31" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
+      <c r="G31" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B32" t="str">
+        <v>80079</v>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
+        <v>17                                                                                   80079</v>
+      </c>
+      <c r="G32" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+      <c r="B33" t="str">
+        <v>80079</v>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E33" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Onroerend goed object 2</v>
+      </c>
+      <c r="B34" t="str">
+        <v>80077 80093 86451</v>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <v>18 Onroerend goed object 2   80077 80093 86451</v>
+      </c>
+      <c r="G34" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v/>
+      </c>
+      <c r="B35" t="str">
+        <v>80077</v>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E35" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v/>
+      </c>
+      <c r="B36" t="str">
+        <v>80093</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E36" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v/>
+      </c>
+      <c r="B37" t="str">
+        <v>86451</v>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E37" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
+      <c r="G37" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B38" t="str">
+        <v>80082 80088</v>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <v/>
+      </c>
+      <c r="F38" t="str">
+        <v>19                           80082 80088</v>
+      </c>
+      <c r="G38" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v/>
+      </c>
+      <c r="B39" t="str">
+        <v>80082</v>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E39" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F39" t="str">
+        <v/>
+      </c>
+      <c r="G39" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v/>
+      </c>
+      <c r="B40" t="str">
+        <v>80088</v>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E40" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
+      <c r="G40" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Dekkingscombinatie</v>
+      </c>
+      <c r="B41" t="str">
+        <v>80733</v>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <v/>
+      </c>
+      <c r="F41" t="str">
+        <v>20 Dekkingscombinatie        80733</v>
+      </c>
+      <c r="G41" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v/>
+      </c>
+      <c r="B42" t="str">
+        <v>80733</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E42" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F42" t="str">
+        <v/>
+      </c>
+      <c r="G42" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Herbouwwaarde</v>
+      </c>
+      <c r="B43" t="str">
+        <v>€ 80735</v>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43" t="str">
+        <v/>
+      </c>
+      <c r="F43" t="str">
+        <v>21 Herbouwwaarde             € 80735</v>
+      </c>
+      <c r="G43" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v/>
+      </c>
+      <c r="B44" t="str">
+        <v>80735</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E44" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F44" t="str">
+        <v/>
+      </c>
+      <c r="G44" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Huurwaarde</v>
+      </c>
+      <c r="B45" t="str">
+        <v>€ 80737</v>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45" t="str">
+        <v/>
+      </c>
+      <c r="F45" t="str">
+        <v>22 Huurwaarde                € 80737</v>
+      </c>
+      <c r="G45" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v/>
+      </c>
+      <c r="B46" t="str">
+        <v>80737</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E46" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F46" t="str">
+        <v/>
+      </c>
+      <c r="G46" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B47" t="str">
+        <v>80077</v>
+      </c>
+      <c r="C47" t="str">
+        <v/>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <v/>
+      </c>
+      <c r="F47" t="str">
+        <v>23                                                                                   80077</v>
+      </c>
+      <c r="G47" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v/>
+      </c>
+      <c r="B48" t="str">
+        <v>80077</v>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E48" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F48" t="str">
+        <v/>
+      </c>
+      <c r="G48" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Onroerend goed object 3</v>
+      </c>
+      <c r="B49" t="str">
+        <v>80078 80094 86577</v>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <v/>
+      </c>
+      <c r="F49" t="str">
+        <v>24 Onroerend goed object 3   80078 80094 86577</v>
+      </c>
+      <c r="G49" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v/>
+      </c>
+      <c r="B50" t="str">
+        <v>80078</v>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E50" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F50" t="str">
+        <v/>
+      </c>
+      <c r="G50" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v/>
+      </c>
+      <c r="B51" t="str">
+        <v>80094</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Getal exclusief decimalen</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E51" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F51" t="str">
+        <v/>
+      </c>
+      <c r="G51" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v/>
+      </c>
+      <c r="B52" t="str">
+        <v>86577</v>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+      <c r="D52" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E52" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F52" t="str">
+        <v/>
+      </c>
+      <c r="G52" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B53" t="str">
+        <v>80083 80089</v>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+      <c r="D53" t="str">
+        <v/>
+      </c>
+      <c r="E53" t="str">
+        <v/>
+      </c>
+      <c r="F53" t="str">
+        <v>25                           80083 80089</v>
+      </c>
+      <c r="G53" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v/>
+      </c>
+      <c r="B54" t="str">
+        <v>80083</v>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+      <c r="D54" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E54" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F54" t="str">
+        <v/>
+      </c>
+      <c r="G54" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v/>
+      </c>
+      <c r="B55" t="str">
+        <v>80089</v>
+      </c>
+      <c r="C55" t="str">
+        <v/>
+      </c>
+      <c r="D55" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E55" t="str">
+        <v>niet verwijderen</v>
+      </c>
+      <c r="F55" t="str">
+        <v/>
+      </c>
+      <c r="G55" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Dekkingscombinatie</v>
+      </c>
+      <c r="B56" t="str">
+        <v>80734</v>
+      </c>
+      <c r="C56" t="str">
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56" t="str">
+        <v/>
+      </c>
+      <c r="F56" t="str">
+        <v>26 Dekkingscombinatie        80734</v>
+      </c>
+      <c r="G56" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v/>
+      </c>
+      <c r="B57" t="str">
+        <v>80734</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Omschrijving</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E57" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F57" t="str">
+        <v/>
+      </c>
+      <c r="G57" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Herbouwwaarde</v>
+      </c>
+      <c r="B58" t="str">
+        <v>€ 80736</v>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <v/>
+      </c>
+      <c r="F58" t="str">
+        <v>27 Herbouwwaarde             € 80736</v>
+      </c>
+      <c r="G58" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v/>
+      </c>
+      <c r="B59" t="str">
+        <v>80736</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E59" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F59" t="str">
+        <v/>
+      </c>
+      <c r="G59" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Huurwaarde</v>
+      </c>
+      <c r="B60" t="str">
+        <v>€ 80738</v>
+      </c>
+      <c r="C60" t="str">
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <v/>
+      </c>
+      <c r="E60" t="str">
+        <v/>
+      </c>
+      <c r="F60" t="str">
+        <v>28 Huurwaarde                € 80738</v>
+      </c>
+      <c r="G60" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v/>
+      </c>
+      <c r="B61" t="str">
+        <v>80738</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Getal inclusief decimalen</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Rechts</v>
+      </c>
+      <c r="E61" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F61" t="str">
+        <v/>
+      </c>
+      <c r="G61" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B62" t="str">
+        <v>80078</v>
+      </c>
+      <c r="C62" t="str">
+        <v/>
+      </c>
+      <c r="D62" t="str">
+        <v/>
+      </c>
+      <c r="E62" t="str">
+        <v/>
+      </c>
+      <c r="F62" t="str">
+        <v>29                                                                                   80078</v>
+      </c>
+      <c r="G62" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v/>
+      </c>
+      <c r="B63" t="str">
+        <v>80078</v>
+      </c>
+      <c r="C63" t="str">
+        <v/>
+      </c>
+      <c r="D63" t="str">
+        <v>Links</v>
+      </c>
+      <c r="E63" t="str">
+        <v>verwijderen</v>
+      </c>
+      <c r="F63" t="str">
+        <v/>
+      </c>
+      <c r="G63" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Geschil</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Als u een juridisch geschil wilt melden of behoefte heeft aan juridisch advies kunt u</v>
+      </c>
+      <c r="C64" t="str">
+        <v/>
+      </c>
+      <c r="D64" t="str">
+        <v/>
+      </c>
+      <c r="E64" t="str">
+        <v/>
+      </c>
+      <c r="F64" t="str">
+        <v>30 Geschil                   Als u een juridisch geschil wilt melden of behoefte heeft aan juridisch advies kunt u</v>
+      </c>
+      <c r="G64" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B65" t="str">
+        <v>contact opnemen met:</v>
+      </c>
+      <c r="C65" t="str">
+        <v/>
+      </c>
+      <c r="D65" t="str">
+        <v/>
+      </c>
+      <c r="E65" t="str">
+        <v/>
+      </c>
+      <c r="F65" t="str">
+        <v>31                           contact opnemen met:</v>
+      </c>
+      <c r="G65" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B66" t="str">
+        <v>ARAG Rechtsbijstand</v>
+      </c>
+      <c r="C66" t="str">
+        <v/>
+      </c>
+      <c r="D66" t="str">
+        <v/>
+      </c>
+      <c r="E66" t="str">
+        <v/>
+      </c>
+      <c r="F66" t="str">
+        <v>32                           ARAG Rechtsbijstand</v>
+      </c>
+      <c r="G66" t="str">
+        <v>x</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="B67" t="str">
+        <v>T (033) - 434 23 42 of via www.ARAG.nl</v>
+      </c>
+      <c r="C67" t="str">
+        <v/>
+      </c>
+      <c r="D67" t="str">
+        <v/>
+      </c>
+      <c r="E67" t="str">
+        <v/>
+      </c>
+      <c r="F67" t="str">
+        <v>33                           T (033) - 434 23 42 of via www.ARAG.nl</v>
+      </c>
+      <c r="G67" t="str">
+        <v>x</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G67"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>